<commit_message>
Update student import file and add new SQL file
</commit_message>
<xml_diff>
--- a/Import Student/omar.xlsx
+++ b/Import Student/omar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECHNICAL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Online_Examntion_System-master\Import Student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18302D7A-4001-4D49-86F0-3D5AA32BAF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F121CB-6E98-4698-9136-7E43C9F85F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>-</t>
   </si>
@@ -52,58 +52,13 @@
     <t>omar@gmail.com</t>
   </si>
   <si>
-    <t>Reem Adel</t>
-  </si>
-  <si>
-    <t>Reem@gmail.com</t>
-  </si>
-  <si>
-    <t>reem123</t>
-  </si>
-  <si>
-    <t>beso@gmail.com</t>
-  </si>
-  <si>
-    <t>beso123</t>
-  </si>
-  <si>
-    <t>Maryam rabi</t>
-  </si>
-  <si>
-    <t>mariam@gmail.com</t>
-  </si>
-  <si>
-    <t>mariam123</t>
-  </si>
-  <si>
-    <t>Elzonfly</t>
-  </si>
-  <si>
-    <t>zonfol@gmail.com</t>
-  </si>
-  <si>
-    <t>zonfol123</t>
-  </si>
-  <si>
-    <t>Maryam Rashad</t>
-  </si>
-  <si>
-    <t>mariamm@gmail.com</t>
-  </si>
-  <si>
-    <t>mariamm123</t>
-  </si>
-  <si>
-    <t>esraa soliman</t>
-  </si>
-  <si>
-    <t>esraa@gmail.com</t>
-  </si>
-  <si>
-    <t>esraa123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bassem </t>
+    <t>Gaber Moahmed</t>
+  </si>
+  <si>
+    <t>Gaber123</t>
+  </si>
+  <si>
+    <t>Gaber Mohamed</t>
   </si>
 </sst>
 </file>
@@ -472,7 +427,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +476,7 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>1276612118</v>
+        <v>1276119111</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -538,109 +493,34 @@
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>1276612119</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>209999999</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>1276619911</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>200000000</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>1279819191</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>201212121</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>12766191919</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>202222222</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>12872891991</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>204444444</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>1277712119</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
+      <c r="C8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{1FED0CC6-1AE0-4435-9A51-8186E747DD1D}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{0EAE738A-2777-43EA-BC21-A3B7F2D792EE}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{8A6924B2-A85D-4B32-BE19-5CE6F78C40B4}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{281B64DC-642D-4B3D-AEEA-2E43AE370A8F}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{84CC0C80-EEB1-484F-AA35-5AD5393835E0}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{1A046A73-CE37-4D14-9CEE-FF829664B0A7}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{702971E9-1B01-45E1-BBE5-74C44B326454}"/>
+    <hyperlink ref="C3" r:id="rId2" display="Reem@gmail.com" xr:uid="{0EAE738A-2777-43EA-BC21-A3B7F2D792EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>